<commit_message>
Add : Notes and code for form, input, select and option tags
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E25F6FAE-C32E-41E8-B2EB-5FFA6D30E472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BB2164-99C2-4C8B-9593-3CB1D09772D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -749,188 +749,188 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C11"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1224,643 +1224,656 @@
     <col min="2" max="2" width="21.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.88671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="59.88671875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="17.21875" style="46" customWidth="1"/>
+    <col min="5" max="5" width="17.21875" style="23" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="45" t="s">
+      <c r="B3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="C3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="D3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="24" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="3"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="48"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="5">
+      <c r="A5" s="49">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="49"/>
+      <c r="E5" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="9"/>
-      <c r="B6" s="10"/>
-      <c r="C6" s="11" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="53" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="D6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="55"/>
+      <c r="E6" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
+      <c r="A7" s="50"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="50"/>
+      <c r="E7" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10"/>
-      <c r="C8" s="15" t="s">
+      <c r="A8" s="50"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="54"/>
+      <c r="E8" s="31"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="16" t="s">
+      <c r="A9" s="50"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="54"/>
+      <c r="E9" s="31"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="16" t="s">
+      <c r="A10" s="50"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="55"/>
+      <c r="E10" s="32"/>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="18"/>
-      <c r="B11" s="19"/>
-      <c r="C11" s="20" t="s">
+      <c r="A11" s="51"/>
+      <c r="B11" s="57"/>
+      <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="51"/>
+      <c r="E11" s="28"/>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="27">
+      <c r="A12" s="43">
         <v>2</v>
       </c>
-      <c r="B12" s="28" t="s">
+      <c r="B12" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="29" t="s">
+      <c r="C12" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="56"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-      <c r="C13" s="32" t="s">
+      <c r="A13" s="44"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="32" t="s">
+      <c r="D13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="57"/>
+      <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-      <c r="C14" s="33" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="34" t="s">
+      <c r="D14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="52"/>
+      <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-      <c r="C15" s="35"/>
-      <c r="D15" s="36" t="s">
+      <c r="A15" s="44"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="58"/>
+      <c r="E15" s="35"/>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-      <c r="C16" s="32" t="s">
+      <c r="A16" s="44"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="32" t="s">
+      <c r="D16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="52"/>
+      <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
-      <c r="C17" s="32" t="s">
+      <c r="A17" s="44"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="32" t="s">
+      <c r="D17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="59"/>
+      <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="32" t="s">
+      <c r="A18" s="44"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="32" t="s">
+      <c r="D18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="59"/>
+      <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="37"/>
-      <c r="B19" s="38"/>
-      <c r="C19" s="39" t="s">
+      <c r="A19" s="45"/>
+      <c r="B19" s="62"/>
+      <c r="C19" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="60"/>
+      <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="22">
+      <c r="A20" s="46">
         <v>3</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="14" t="s">
+      <c r="C20" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="23" t="s">
+      <c r="D20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="61"/>
+      <c r="E20" s="38"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="24"/>
-      <c r="B21" s="9"/>
-      <c r="C21" s="17" t="s">
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="25" t="s">
+      <c r="D21" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="50"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="24"/>
-      <c r="B22" s="9"/>
-      <c r="C22" s="17" t="s">
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="25" t="s">
+      <c r="D22" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="55"/>
+      <c r="E22" s="32"/>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="24"/>
-      <c r="B23" s="9"/>
-      <c r="C23" s="17" t="s">
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="17" t="s">
+      <c r="D23" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="55"/>
+      <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="24"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="17" t="s">
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="25" t="s">
+      <c r="D24" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="55"/>
+      <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="24"/>
-      <c r="B25" s="9"/>
-      <c r="C25" s="17" t="s">
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D25" s="25" t="s">
+      <c r="D25" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="50"/>
+      <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="24"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="17" t="s">
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="E26" s="55"/>
+      <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="24"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="17" t="s">
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="17" t="s">
+      <c r="D27" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E27" s="55"/>
+      <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="26"/>
-      <c r="B28" s="18"/>
-      <c r="C28" s="21" t="s">
+      <c r="A28" s="48"/>
+      <c r="B28" s="51"/>
+      <c r="C28" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="E28" s="51"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="41">
+      <c r="A29" s="40">
         <v>4</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="43" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D29" s="29" t="s">
+      <c r="D29" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="56"/>
+      <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="42"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="32" t="s">
+      <c r="A30" s="41"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D30" s="32" t="s">
+      <c r="D30" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E30" s="52"/>
+      <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="42"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="32" t="s">
+      <c r="A31" s="41"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E31" s="57"/>
+      <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="42"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="32" t="s">
+      <c r="A32" s="41"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="D32" s="32" t="s">
+      <c r="D32" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E32" s="52"/>
+      <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="42"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="32" t="s">
+      <c r="A33" s="41"/>
+      <c r="B33" s="44"/>
+      <c r="C33" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="D33" s="32" t="s">
+      <c r="D33" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="E33" s="57"/>
+      <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="43"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="40" t="s">
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
+      <c r="C34" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="D34" s="40" t="s">
+      <c r="D34" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E34" s="53"/>
+      <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="22">
+      <c r="A35" s="46">
         <v>5</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="D35" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="49"/>
+      <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="24"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="17" t="s">
+      <c r="A36" s="47"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="D36" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="54"/>
+      <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="24"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="17" t="s">
+      <c r="A37" s="47"/>
+      <c r="B37" s="50"/>
+      <c r="C37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="D37" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="55"/>
+      <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="24"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="17" t="s">
+      <c r="A38" s="47"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="17" t="s">
+      <c r="D38" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="50"/>
+      <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="24"/>
-      <c r="B39" s="9"/>
-      <c r="C39" s="17" t="s">
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
+      <c r="C39" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="17" t="s">
+      <c r="D39" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="54"/>
+      <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="24"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="17" t="s">
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
+      <c r="C40" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="17" t="s">
+      <c r="D40" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="54"/>
+      <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="24"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="17" t="s">
+      <c r="A41" s="47"/>
+      <c r="B41" s="50"/>
+      <c r="C41" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="17" t="s">
+      <c r="D41" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="54"/>
+      <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="24"/>
-      <c r="B42" s="9"/>
-      <c r="C42" s="17" t="s">
+      <c r="A42" s="47"/>
+      <c r="B42" s="50"/>
+      <c r="C42" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="17" t="s">
+      <c r="D42" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="54"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="26"/>
-      <c r="B43" s="18"/>
-      <c r="C43" s="21" t="s">
+      <c r="A43" s="48"/>
+      <c r="B43" s="51"/>
+      <c r="C43" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="62"/>
+      <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="41">
+      <c r="A44" s="40">
         <v>6</v>
       </c>
-      <c r="B44" s="27" t="s">
+      <c r="B44" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="29" t="s">
+      <c r="C44" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="29" t="s">
+      <c r="D44" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="E44" s="56"/>
+      <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="42"/>
-      <c r="B45" s="30"/>
-      <c r="C45" s="32" t="s">
+      <c r="A45" s="41"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="32" t="s">
+      <c r="D45" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="52"/>
+      <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="42"/>
-      <c r="B46" s="30"/>
-      <c r="C46" s="32" t="s">
+      <c r="A46" s="41"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="32" t="s">
+      <c r="D46" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="59"/>
+      <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="42"/>
-      <c r="B47" s="30"/>
-      <c r="C47" s="32" t="s">
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="32" t="s">
+      <c r="D47" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="E47" s="57"/>
+      <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="43"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="39" t="s">
+      <c r="A48" s="42"/>
+      <c r="B48" s="45"/>
+      <c r="C48" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D48" s="40" t="s">
+      <c r="D48" s="20" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="53"/>
+      <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="22">
+      <c r="A49" s="46">
         <v>7</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="8" t="s">
+      <c r="C49" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D49" s="8" t="s">
+      <c r="D49" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="49"/>
+      <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="24"/>
-      <c r="B50" s="9"/>
-      <c r="C50" s="17" t="s">
+      <c r="A50" s="47"/>
+      <c r="B50" s="50"/>
+      <c r="C50" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D50" s="17" t="s">
+      <c r="D50" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E50" s="55"/>
+      <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="24"/>
-      <c r="B51" s="9"/>
-      <c r="C51" s="17" t="s">
+      <c r="A51" s="47"/>
+      <c r="B51" s="50"/>
+      <c r="C51" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D51" s="17" t="s">
+      <c r="D51" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="55"/>
+      <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="24"/>
-      <c r="B52" s="9"/>
-      <c r="C52" s="14" t="s">
+      <c r="A52" s="47"/>
+      <c r="B52" s="50"/>
+      <c r="C52" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="14" t="s">
+      <c r="D52" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="50"/>
+      <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="24"/>
-      <c r="B53" s="9"/>
-      <c r="C53" s="17" t="s">
+      <c r="A53" s="47"/>
+      <c r="B53" s="50"/>
+      <c r="C53" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D53" s="17" t="s">
+      <c r="D53" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="55"/>
+      <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="24"/>
-      <c r="B54" s="9"/>
-      <c r="C54" s="17" t="s">
+      <c r="A54" s="47"/>
+      <c r="B54" s="50"/>
+      <c r="C54" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="17" t="s">
+      <c r="D54" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E54" s="50"/>
+      <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="24"/>
-      <c r="B55" s="9"/>
-      <c r="C55" s="17" t="s">
+      <c r="A55" s="47"/>
+      <c r="B55" s="50"/>
+      <c r="C55" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="17" t="s">
+      <c r="D55" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="54"/>
+      <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="26"/>
-      <c r="B56" s="18"/>
-      <c r="C56" s="21" t="s">
+      <c r="A56" s="48"/>
+      <c r="B56" s="51"/>
+      <c r="C56" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="D56" s="21" t="s">
+      <c r="D56" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="E56" s="62"/>
+      <c r="E56" s="39"/>
     </row>
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1871,13 +1884,6 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes for Semantic HTML, attributes, Meta tags, embedded content
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BB2164-99C2-4C8B-9593-3CB1D09772D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3C8EED-0A46-4405-B476-C62A5FD08FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,42 +863,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -917,6 +881,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -930,6 +903,33 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49">
+      <c r="A5" s="46">
         <v>1</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,54 +1304,62 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="31"/>
+      <c r="E9" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="32"/>
+      <c r="E10" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="51"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="E11" s="28"/>
+      <c r="E11" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="54">
         <v>2</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="51" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1363,8 +1371,8 @@
       <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1374,9 +1382,9 @@
       <c r="E13" s="34"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="58" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="49" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1385,17 +1393,17 @@
       <c r="E14" s="29"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
       <c r="E15" s="35"/>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1405,8 +1413,8 @@
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1416,8 +1424,8 @@
       <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1427,8 +1435,8 @@
       <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45"/>
-      <c r="B19" s="62"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="19" t="s">
         <v>34</v>
       </c>
@@ -1438,10 +1446,10 @@
       <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
+      <c r="A20" s="60">
         <v>3</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="46" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1453,8 +1461,8 @@
       <c r="E20" s="38"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
@@ -1464,8 +1472,8 @@
       <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="10" t="s">
         <v>41</v>
       </c>
@@ -1475,8 +1483,8 @@
       <c r="E22" s="32"/>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
@@ -1486,8 +1494,8 @@
       <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="10" t="s">
         <v>45</v>
       </c>
@@ -1497,8 +1505,8 @@
       <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="10" t="s">
         <v>46</v>
       </c>
@@ -1508,8 +1516,8 @@
       <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="10" t="s">
         <v>47</v>
       </c>
@@ -1519,8 +1527,8 @@
       <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="10" t="s">
         <v>49</v>
       </c>
@@ -1530,8 +1538,8 @@
       <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="48"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="12" t="s">
         <v>51</v>
       </c>
@@ -1541,10 +1549,10 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40">
+      <c r="A29" s="57">
         <v>4</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="54" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1556,8 +1564,8 @@
       <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="16" t="s">
         <v>56</v>
       </c>
@@ -1567,8 +1575,8 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="16" t="s">
         <v>59</v>
       </c>
@@ -1578,8 +1586,8 @@
       <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="16" t="s">
         <v>61</v>
       </c>
@@ -1589,8 +1597,8 @@
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="16" t="s">
         <v>63</v>
       </c>
@@ -1600,8 +1608,8 @@
       <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="20" t="s">
         <v>66</v>
       </c>
@@ -1611,10 +1619,10 @@
       <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="60">
         <v>5</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="46" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1626,8 +1634,8 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="10" t="s">
         <v>56</v>
       </c>
@@ -1637,8 +1645,8 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="10" t="s">
         <v>71</v>
       </c>
@@ -1648,8 +1656,8 @@
       <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="50"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="10" t="s">
         <v>73</v>
       </c>
@@ -1659,8 +1667,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="10" t="s">
         <v>75</v>
       </c>
@@ -1670,8 +1678,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="10" t="s">
         <v>77</v>
       </c>
@@ -1681,8 +1689,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="10" t="s">
         <v>79</v>
       </c>
@@ -1692,8 +1700,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="10" t="s">
         <v>81</v>
       </c>
@@ -1703,8 +1711,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="12" t="s">
         <v>83</v>
       </c>
@@ -1714,10 +1722,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40">
+      <c r="A44" s="57">
         <v>6</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="54" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1729,8 +1737,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="41"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="16" t="s">
         <v>88</v>
       </c>
@@ -1740,8 +1748,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="41"/>
-      <c r="B46" s="44"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="16" t="s">
         <v>90</v>
       </c>
@@ -1751,8 +1759,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="41"/>
-      <c r="B47" s="44"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="16" t="s">
         <v>92</v>
       </c>
@@ -1762,8 +1770,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="42"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="59"/>
+      <c r="B48" s="56"/>
       <c r="C48" s="19" t="s">
         <v>94</v>
       </c>
@@ -1773,10 +1781,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="46">
+      <c r="A49" s="60">
         <v>7</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="46" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1788,8 +1796,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="47"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="10" t="s">
         <v>99</v>
       </c>
@@ -1799,8 +1807,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
-      <c r="B51" s="50"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="10" t="s">
         <v>101</v>
       </c>
@@ -1810,8 +1818,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="47"/>
-      <c r="B52" s="50"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="47"/>
       <c r="C52" s="7" t="s">
         <v>103</v>
       </c>
@@ -1821,8 +1829,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="47"/>
-      <c r="B53" s="50"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="10" t="s">
         <v>105</v>
       </c>
@@ -1832,8 +1840,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="50"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="47"/>
       <c r="C54" s="10" t="s">
         <v>107</v>
       </c>
@@ -1843,8 +1851,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="50"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="47"/>
       <c r="C55" s="10" t="s">
         <v>109</v>
       </c>
@@ -1854,8 +1862,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="48"/>
-      <c r="B56" s="51"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="12" t="s">
         <v>111</v>
       </c>
@@ -1867,13 +1875,6 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1884,6 +1885,13 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes on Selectors, Box Model, Flexbox & Grid layout techniques
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A3C8EED-0A46-4405-B476-C62A5FD08FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1625897-664A-440F-8D75-D3455AFF889D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -881,15 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -903,33 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46">
+      <c r="A5" s="49">
         <v>1</v>
       </c>
-      <c r="B5" s="43" t="s">
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="41" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="47"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="48"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="43">
         <v>2</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="60" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1368,42 +1368,50 @@
       <c r="D12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="E12" s="33"/>
+      <c r="E12" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="58" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="29"/>
+      <c r="E14" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E15" s="35"/>
+      <c r="E15" s="35">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1413,8 +1421,8 @@
       <c r="E16" s="29"/>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1424,8 +1432,8 @@
       <c r="E17" s="36"/>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="55"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1435,8 +1443,8 @@
       <c r="E18" s="36"/>
     </row>
     <row r="19" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="56"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="19" t="s">
         <v>34</v>
       </c>
@@ -1446,10 +1454,10 @@
       <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="60">
+      <c r="A20" s="46">
         <v>3</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="49" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1461,8 +1469,8 @@
       <c r="E20" s="38"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
@@ -1472,8 +1480,8 @@
       <c r="E21" s="27"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="61"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="10" t="s">
         <v>41</v>
       </c>
@@ -1483,8 +1491,8 @@
       <c r="E22" s="32"/>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="61"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="10" t="s">
         <v>43</v>
       </c>
@@ -1494,8 +1502,8 @@
       <c r="E23" s="32"/>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="47"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="10" t="s">
         <v>45</v>
       </c>
@@ -1505,8 +1513,8 @@
       <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="10" t="s">
         <v>46</v>
       </c>
@@ -1516,8 +1524,8 @@
       <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="10" t="s">
         <v>47</v>
       </c>
@@ -1527,8 +1535,8 @@
       <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="10" t="s">
         <v>49</v>
       </c>
@@ -1538,8 +1546,8 @@
       <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="62"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="12" t="s">
         <v>51</v>
       </c>
@@ -1549,10 +1557,10 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="57">
+      <c r="A29" s="40">
         <v>4</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="43" t="s">
         <v>53</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1564,8 +1572,8 @@
       <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="58"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="16" t="s">
         <v>56</v>
       </c>
@@ -1575,8 +1583,8 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="16" t="s">
         <v>59</v>
       </c>
@@ -1586,8 +1594,8 @@
       <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="58"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="16" t="s">
         <v>61</v>
       </c>
@@ -1597,8 +1605,8 @@
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="16" t="s">
         <v>63</v>
       </c>
@@ -1608,8 +1616,8 @@
       <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="59"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="20" t="s">
         <v>66</v>
       </c>
@@ -1619,10 +1627,10 @@
       <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="60">
+      <c r="A35" s="46">
         <v>5</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="49" t="s">
         <v>68</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1634,8 +1642,8 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="61"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="10" t="s">
         <v>56</v>
       </c>
@@ -1645,8 +1653,8 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="61"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="10" t="s">
         <v>71</v>
       </c>
@@ -1656,8 +1664,8 @@
       <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="61"/>
-      <c r="B38" s="47"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="10" t="s">
         <v>73</v>
       </c>
@@ -1667,8 +1675,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="61"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="10" t="s">
         <v>75</v>
       </c>
@@ -1678,8 +1686,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="61"/>
-      <c r="B40" s="47"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="10" t="s">
         <v>77</v>
       </c>
@@ -1689,8 +1697,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="61"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="10" t="s">
         <v>79</v>
       </c>
@@ -1700,8 +1708,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="61"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="10" t="s">
         <v>81</v>
       </c>
@@ -1711,8 +1719,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="62"/>
-      <c r="B43" s="48"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="12" t="s">
         <v>83</v>
       </c>
@@ -1722,10 +1730,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="57">
+      <c r="A44" s="40">
         <v>6</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="43" t="s">
         <v>85</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1737,8 +1745,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="58"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="16" t="s">
         <v>88</v>
       </c>
@@ -1748,8 +1756,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="55"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="44"/>
       <c r="C46" s="16" t="s">
         <v>90</v>
       </c>
@@ -1759,8 +1767,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="58"/>
-      <c r="B47" s="55"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="16" t="s">
         <v>92</v>
       </c>
@@ -1770,8 +1778,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="59"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="19" t="s">
         <v>94</v>
       </c>
@@ -1781,10 +1789,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="60">
+      <c r="A49" s="46">
         <v>7</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="49" t="s">
         <v>96</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1796,8 +1804,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="61"/>
-      <c r="B50" s="47"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="10" t="s">
         <v>99</v>
       </c>
@@ -1807,8 +1815,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="61"/>
-      <c r="B51" s="47"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="50"/>
       <c r="C51" s="10" t="s">
         <v>101</v>
       </c>
@@ -1818,8 +1826,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="61"/>
-      <c r="B52" s="47"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="7" t="s">
         <v>103</v>
       </c>
@@ -1829,8 +1837,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="61"/>
-      <c r="B53" s="47"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="10" t="s">
         <v>105</v>
       </c>
@@ -1840,8 +1848,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="61"/>
-      <c r="B54" s="47"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="10" t="s">
         <v>107</v>
       </c>
@@ -1851,8 +1859,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="61"/>
-      <c r="B55" s="47"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="10" t="s">
         <v>109</v>
       </c>
@@ -1862,8 +1870,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="62"/>
-      <c r="B56" s="48"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="12" t="s">
         <v>111</v>
       </c>
@@ -1875,6 +1883,13 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1885,13 +1900,6 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes for Positioning, Typography, Colors, Backgrounds & Common properties and Media Query Syntax
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1625897-664A-440F-8D75-D3455AFF889D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90098C7-1649-446A-AA78-5CF907F85D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -132,9 +132,6 @@
     <t>color denoting types, background, display types</t>
   </si>
   <si>
-    <t>Styling Forms &amp; Responsive Design</t>
-  </si>
-  <si>
     <t>input fields and buttons, media queries syntax</t>
   </si>
   <si>
@@ -368,6 +365,9 @@
   </si>
   <si>
     <t>handling errors using error boundaries in component trees</t>
+  </si>
+  <si>
+    <t>Media Query Syntax</t>
   </si>
 </sst>
 </file>
@@ -863,6 +863,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,15 +923,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,48 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49">
+      <c r="A5" s="46">
         <v>1</v>
       </c>
-      <c r="B5" s="55" t="s">
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="51"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="54">
         <v>2</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="51" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="58" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="49" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,486 +1410,487 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="29"/>
+      <c r="E16" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="D17" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
       <c r="D18" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="E18" s="36"/>
-    </row>
-    <row r="19" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45"/>
-      <c r="B19" s="62"/>
+      <c r="E18" s="36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="56"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="20" t="s">
+      <c r="E19" s="37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="60">
+        <v>3</v>
+      </c>
+      <c r="B20" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="E19" s="37"/>
-    </row>
-    <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
-        <v>3</v>
-      </c>
-      <c r="B20" s="49" t="s">
+      <c r="C20" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="13" t="s">
+      <c r="E20" s="38"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="61"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="38"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
-      <c r="C21" s="10" t="s">
+      <c r="D21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="E21" s="27"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="61"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E21" s="27"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
-      <c r="C22" s="10" t="s">
+      <c r="D22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="E22" s="32"/>
+    </row>
+    <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A23" s="61"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E22" s="32"/>
-    </row>
-    <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
-      <c r="C23" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D23" s="10" t="s">
+      <c r="E23" s="32"/>
+    </row>
+    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A24" s="61"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="E23" s="32"/>
-    </row>
-    <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
-      <c r="C24" s="10" t="s">
+      <c r="D24" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="32"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="61"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D25" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="E25" s="27"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="61"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="32"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="61"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="32"/>
+    </row>
+    <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="62"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E28" s="28"/>
+    </row>
+    <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="57">
+        <v>4</v>
+      </c>
+      <c r="B29" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D29" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" s="33"/>
+    </row>
+    <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="D30" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E24" s="32"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D25" s="14" t="s">
+      <c r="E30" s="29"/>
+    </row>
+    <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A31" s="58"/>
+      <c r="B31" s="55"/>
+      <c r="C31" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D31" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="E31" s="34"/>
+    </row>
+    <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
+      <c r="C32" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="E32" s="29"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D33" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33" s="34"/>
+    </row>
+    <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="59"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="27"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
-      <c r="C26" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E26" s="32"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
-      <c r="C27" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E27" s="32"/>
-    </row>
-    <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="48"/>
-      <c r="B28" s="51"/>
-      <c r="C28" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="D28" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="E28" s="28"/>
-    </row>
-    <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40">
-        <v>4</v>
-      </c>
-      <c r="B29" s="43" t="s">
+      <c r="D34" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E34" s="30"/>
+    </row>
+    <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="60">
+        <v>5</v>
+      </c>
+      <c r="B35" s="46" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C29" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="D29" s="15" t="s">
+      <c r="D35" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E35" s="26"/>
+    </row>
+    <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="A36" s="61"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E29" s="33"/>
-    </row>
-    <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
-      <c r="C30" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E30" s="29"/>
-    </row>
-    <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D31" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="E31" s="34"/>
-    </row>
-    <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="16" t="s">
-        <v>61</v>
-      </c>
-      <c r="D32" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E32" s="29"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="D33" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E33" s="34"/>
-    </row>
-    <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
-      <c r="C34" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" s="30"/>
-    </row>
-    <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
-        <v>5</v>
-      </c>
-      <c r="B35" s="49" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D35" s="5" t="s">
+      <c r="D36" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E35" s="26"/>
-    </row>
-    <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="50"/>
-      <c r="C36" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="D36" s="10" t="s">
+      <c r="E36" s="31"/>
+    </row>
+    <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
+      <c r="A37" s="61"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="E36" s="31"/>
-    </row>
-    <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50"/>
-      <c r="C37" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="D37" s="10" t="s">
+      <c r="E37" s="32"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="61"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E37" s="32"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="50"/>
-      <c r="C38" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="D38" s="10" t="s">
+      <c r="E38" s="27"/>
+    </row>
+    <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A39" s="61"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="27"/>
-    </row>
-    <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
-      <c r="C39" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="E39" s="31"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="E39" s="31"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
-      <c r="C40" s="10" t="s">
+      <c r="D40" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="10" t="s">
+      <c r="E40" s="31"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="61"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="E40" s="31"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="10" t="s">
+      <c r="D41" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="D41" s="10" t="s">
+      <c r="E41" s="31"/>
+    </row>
+    <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A42" s="61"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E41" s="31"/>
-    </row>
-    <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="50"/>
-      <c r="C42" s="10" t="s">
+      <c r="D42" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="31"/>
+    </row>
+    <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="62"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E42" s="31"/>
-    </row>
-    <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="51"/>
-      <c r="C43" s="12" t="s">
+      <c r="D43" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="E43" s="39"/>
+    </row>
+    <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="57">
+        <v>6</v>
+      </c>
+      <c r="B44" s="54" t="s">
         <v>84</v>
       </c>
-      <c r="E43" s="39"/>
-    </row>
-    <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40">
-        <v>6</v>
-      </c>
-      <c r="B44" s="43" t="s">
+      <c r="C44" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C44" s="15" t="s">
+      <c r="D44" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="E44" s="33"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
+      <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="E44" s="33"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="41"/>
-      <c r="B45" s="44"/>
-      <c r="C45" s="16" t="s">
+      <c r="D45" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="D45" s="16" t="s">
+      <c r="E45" s="29"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
+      <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="E45" s="29"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="41"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="16" t="s">
+      <c r="D46" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="D46" s="16" t="s">
+      <c r="E46" s="36"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
+      <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="E46" s="36"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="41"/>
-      <c r="B47" s="44"/>
-      <c r="C47" s="16" t="s">
+      <c r="D47" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="E47" s="34"/>
+    </row>
+    <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="59"/>
+      <c r="B48" s="56"/>
+      <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="E47" s="34"/>
-    </row>
-    <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="42"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="19" t="s">
+      <c r="D48" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="E48" s="30"/>
+    </row>
+    <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="60">
+        <v>7</v>
+      </c>
+      <c r="B49" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="30"/>
-    </row>
-    <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="46">
-        <v>7</v>
-      </c>
-      <c r="B49" s="49" t="s">
+      <c r="C49" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="D49" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="E49" s="26"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="61"/>
+      <c r="B50" s="47"/>
+      <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="26"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="47"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="D50" s="10" t="s">
+      <c r="E50" s="32"/>
+    </row>
+    <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A51" s="61"/>
+      <c r="B51" s="47"/>
+      <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="E50" s="32"/>
-    </row>
-    <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
-      <c r="B51" s="50"/>
-      <c r="C51" s="10" t="s">
+      <c r="D51" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="E51" s="32"/>
+    </row>
+    <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A52" s="61"/>
+      <c r="B52" s="47"/>
+      <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="E51" s="32"/>
-    </row>
-    <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="47"/>
-      <c r="B52" s="50"/>
-      <c r="C52" s="7" t="s">
+      <c r="D52" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="E52" s="27"/>
+    </row>
+    <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A53" s="61"/>
+      <c r="B53" s="47"/>
+      <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="27"/>
-    </row>
-    <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="47"/>
-      <c r="B53" s="50"/>
-      <c r="C53" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="D53" s="10" t="s">
+      <c r="E53" s="32"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A54" s="61"/>
+      <c r="B54" s="47"/>
+      <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E53" s="32"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="50"/>
-      <c r="C54" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D54" s="10" t="s">
+      <c r="E54" s="27"/>
+    </row>
+    <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+      <c r="A55" s="61"/>
+      <c r="B55" s="47"/>
+      <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E54" s="27"/>
-    </row>
-    <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="50"/>
-      <c r="C55" s="10" t="s">
+      <c r="D55" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="E55" s="31"/>
+    </row>
+    <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A56" s="62"/>
+      <c r="B56" s="48"/>
+      <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
-      <c r="E55" s="31"/>
-    </row>
-    <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="48"/>
-      <c r="B56" s="51"/>
-      <c r="C56" s="12" t="s">
+      <c r="D56" s="12" t="s">
         <v>111</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>112</v>
       </c>
       <c r="E56" s="39"/>
     </row>
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1900,6 +1901,13 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes for Basics, Control statements and functions of JavaScript
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90098C7-1649-446A-AA78-5CF907F85D38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9C6B96-ACF1-4844-AFBC-7C74E24A925E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1474,7 +1474,9 @@
       <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="38"/>
+      <c r="E20" s="38">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="61"/>
@@ -1485,7 +1487,9 @@
       <c r="D21" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="27"/>
+      <c r="E21" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="61"/>
@@ -1496,7 +1500,9 @@
       <c r="D22" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="32"/>
+      <c r="E22" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A23" s="61"/>

</xml_diff>

<commit_message>
Add : Notes for DOM Manipulation, Event listeners and Event delegation
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D9C6B96-ACF1-4844-AFBC-7C74E24A925E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C9E2D-FE01-4326-9AA6-B339F6D523B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -881,15 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -903,33 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46">
-        <v>1</v>
-      </c>
-      <c r="B5" s="43" t="s">
+      <c r="A5" s="49">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="41" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="47"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="48"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="43">
         <v>2</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="60" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="58" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="55"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="56"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="60">
+      <c r="A20" s="46">
         <v>3</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="49" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="61"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,19 +1505,21 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="61"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="E23" s="32"/>
+      <c r="E23" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="47"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1527,8 +1529,8 @@
       <c r="E24" s="32"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1538,8 +1540,8 @@
       <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1549,8 +1551,8 @@
       <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1560,8 +1562,8 @@
       <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="62"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
@@ -1571,10 +1573,10 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="57">
+      <c r="A29" s="40">
         <v>4</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1586,8 +1588,8 @@
       <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="58"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1597,8 +1599,8 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
@@ -1608,8 +1610,8 @@
       <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="58"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
@@ -1619,8 +1621,8 @@
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1630,8 +1632,8 @@
       <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="59"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
@@ -1641,10 +1643,10 @@
       <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="60">
+      <c r="A35" s="46">
         <v>5</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="49" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1656,8 +1658,8 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="61"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1667,8 +1669,8 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="61"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
@@ -1678,8 +1680,8 @@
       <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="61"/>
-      <c r="B38" s="47"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
@@ -1689,8 +1691,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="61"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
@@ -1700,8 +1702,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="61"/>
-      <c r="B40" s="47"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
@@ -1711,8 +1713,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="61"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1722,8 +1724,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="61"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1733,8 +1735,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="62"/>
-      <c r="B43" s="48"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1744,10 +1746,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="57">
+      <c r="A44" s="40">
         <v>6</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="43" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1759,8 +1761,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="58"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1770,8 +1772,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="55"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="44"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
@@ -1781,8 +1783,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="58"/>
-      <c r="B47" s="55"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1792,8 +1794,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="59"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1803,10 +1805,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="60">
+      <c r="A49" s="46">
         <v>7</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="49" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1818,8 +1820,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="61"/>
-      <c r="B50" s="47"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1829,8 +1831,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="61"/>
-      <c r="B51" s="47"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="50"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1840,8 +1842,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="61"/>
-      <c r="B52" s="47"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1851,8 +1853,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="61"/>
-      <c r="B53" s="47"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1862,8 +1864,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="61"/>
-      <c r="B54" s="47"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1873,8 +1875,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="61"/>
-      <c r="B55" s="47"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1884,8 +1886,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="62"/>
-      <c r="B56" s="48"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1897,6 +1899,13 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1907,13 +1916,6 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : ES6 features notes
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{398C9E2D-FE01-4326-9AA6-B339F6D523B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAA75A2-70FC-4DBC-9113-7B32D0E1CA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,15 +923,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,48 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49">
-        <v>1</v>
-      </c>
-      <c r="B5" s="55" t="s">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="51"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="54">
         <v>2</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="51" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="58" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="49" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45"/>
-      <c r="B19" s="62"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
+      <c r="A20" s="60">
         <v>3</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,8 +1505,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1518,19 +1518,21 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="E24" s="32"/>
+      <c r="E24" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1540,8 +1542,8 @@
       <c r="E25" s="27"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1551,8 +1553,8 @@
       <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1562,8 +1564,8 @@
       <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="48"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
@@ -1573,10 +1575,10 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40">
+      <c r="A29" s="57">
         <v>4</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="54" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1588,8 +1590,8 @@
       <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1599,8 +1601,8 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
@@ -1610,8 +1612,8 @@
       <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
@@ -1621,8 +1623,8 @@
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1632,8 +1634,8 @@
       <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
@@ -1643,10 +1645,10 @@
       <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="60">
         <v>5</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="46" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1658,8 +1660,8 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1669,8 +1671,8 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
@@ -1680,8 +1682,8 @@
       <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="50"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
@@ -1691,8 +1693,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
@@ -1702,8 +1704,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
@@ -1713,8 +1715,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1724,8 +1726,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1735,8 +1737,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1746,10 +1748,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40">
+      <c r="A44" s="57">
         <v>6</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="54" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1761,8 +1763,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="41"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1772,8 +1774,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="41"/>
-      <c r="B46" s="44"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
@@ -1783,8 +1785,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="41"/>
-      <c r="B47" s="44"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1794,8 +1796,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="42"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="59"/>
+      <c r="B48" s="56"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1805,10 +1807,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="46">
+      <c r="A49" s="60">
         <v>7</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="46" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1820,8 +1822,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="47"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1831,8 +1833,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
-      <c r="B51" s="50"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1842,8 +1844,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="47"/>
-      <c r="B52" s="50"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="47"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1853,8 +1855,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="47"/>
-      <c r="B53" s="50"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1864,8 +1866,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="50"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="47"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1875,8 +1877,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="50"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="47"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1886,8 +1888,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="48"/>
-      <c r="B56" s="51"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1899,13 +1901,6 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1916,6 +1911,13 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Asynchronous Programming notes and code
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDAA75A2-70FC-4DBC-9113-7B32D0E1CA60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB922C00-66E7-4206-A083-19912CD02928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -881,15 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -903,33 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46">
-        <v>1</v>
-      </c>
-      <c r="B5" s="43" t="s">
+      <c r="A5" s="49">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="41" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="47"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="48"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="43">
         <v>2</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="60" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="58" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="55"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="56"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="60">
+      <c r="A20" s="46">
         <v>3</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="49" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="61"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,8 +1505,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="61"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1518,8 +1518,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="47"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1531,19 +1531,21 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="27"/>
+      <c r="E25" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1553,8 +1555,8 @@
       <c r="E26" s="32"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1564,8 +1566,8 @@
       <c r="E27" s="32"/>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="62"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
@@ -1575,10 +1577,10 @@
       <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="57">
+      <c r="A29" s="40">
         <v>4</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1590,8 +1592,8 @@
       <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="58"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1601,8 +1603,8 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
@@ -1612,8 +1614,8 @@
       <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="58"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
@@ -1623,8 +1625,8 @@
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1634,8 +1636,8 @@
       <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="59"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
@@ -1645,10 +1647,10 @@
       <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="60">
+      <c r="A35" s="46">
         <v>5</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="49" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1660,8 +1662,8 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="61"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1671,8 +1673,8 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="61"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
@@ -1682,8 +1684,8 @@
       <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="61"/>
-      <c r="B38" s="47"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
@@ -1693,8 +1695,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="61"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
@@ -1704,8 +1706,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="61"/>
-      <c r="B40" s="47"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
@@ -1715,8 +1717,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="61"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1726,8 +1728,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="61"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1737,8 +1739,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="62"/>
-      <c r="B43" s="48"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1748,10 +1750,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="57">
+      <c r="A44" s="40">
         <v>6</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="43" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1763,8 +1765,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="58"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1774,8 +1776,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="55"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="44"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
@@ -1785,8 +1787,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="58"/>
-      <c r="B47" s="55"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1796,8 +1798,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="59"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1807,10 +1809,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="60">
+      <c r="A49" s="46">
         <v>7</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="49" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1822,8 +1824,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="61"/>
-      <c r="B50" s="47"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1833,8 +1835,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="61"/>
-      <c r="B51" s="47"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="50"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1844,8 +1846,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="61"/>
-      <c r="B52" s="47"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1855,8 +1857,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="61"/>
-      <c r="B53" s="47"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1866,8 +1868,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="61"/>
-      <c r="B54" s="47"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1877,8 +1879,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="61"/>
-      <c r="B55" s="47"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1888,8 +1890,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="62"/>
-      <c r="B56" s="48"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1901,6 +1903,13 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1911,13 +1920,6 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes for JSON, Common built in functions and FetchAPI
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB922C00-66E7-4206-A083-19912CD02928}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC547FC4-A298-4F92-A90C-4550829C3ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,15 +923,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,48 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49">
-        <v>1</v>
-      </c>
-      <c r="B5" s="55" t="s">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="51"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="54">
         <v>2</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="51" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="58" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="49" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45"/>
-      <c r="B19" s="62"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
+      <c r="A20" s="60">
         <v>3</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,8 +1505,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1518,8 +1518,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1531,8 +1531,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1544,43 +1544,49 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="32"/>
+      <c r="E26" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E27" s="32"/>
+      <c r="E27" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="48"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E28" s="28"/>
+      <c r="E28" s="28">
+        <v>1</v>
+      </c>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40">
+      <c r="A29" s="57">
         <v>4</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="54" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1592,8 +1598,8 @@
       <c r="E29" s="33"/>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1603,8 +1609,8 @@
       <c r="E30" s="29"/>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
@@ -1614,8 +1620,8 @@
       <c r="E31" s="34"/>
     </row>
     <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
@@ -1625,8 +1631,8 @@
       <c r="E32" s="29"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1636,8 +1642,8 @@
       <c r="E33" s="34"/>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
@@ -1647,10 +1653,10 @@
       <c r="E34" s="30"/>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="60">
         <v>5</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="46" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1662,8 +1668,8 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1673,8 +1679,8 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
@@ -1684,8 +1690,8 @@
       <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="50"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
@@ -1695,8 +1701,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
@@ -1706,8 +1712,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
@@ -1717,8 +1723,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1728,8 +1734,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1739,8 +1745,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1750,10 +1756,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40">
+      <c r="A44" s="57">
         <v>6</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="54" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1765,8 +1771,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="41"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1776,8 +1782,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="41"/>
-      <c r="B46" s="44"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
@@ -1787,8 +1793,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="41"/>
-      <c r="B47" s="44"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1798,8 +1804,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="42"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="59"/>
+      <c r="B48" s="56"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1809,10 +1815,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="46">
+      <c r="A49" s="60">
         <v>7</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="46" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1824,8 +1830,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="47"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1835,8 +1841,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
-      <c r="B51" s="50"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1846,8 +1852,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="47"/>
-      <c r="B52" s="50"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="47"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1857,8 +1863,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="47"/>
-      <c r="B53" s="50"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1868,8 +1874,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="50"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="47"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1879,8 +1885,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="50"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="47"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1890,8 +1896,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="48"/>
-      <c r="B56" s="51"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1903,13 +1909,6 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1920,6 +1919,13 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes and code for node js
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC547FC4-A298-4F92-A90C-4550829C3ED9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E513E3-D17F-4B7C-A395-7B0B3171AF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1595,7 +1595,9 @@
       <c r="D29" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E29" s="33"/>
+      <c r="E29" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
       <c r="A30" s="58"/>
@@ -1606,7 +1608,9 @@
       <c r="D30" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E30" s="29"/>
+      <c r="E30" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
       <c r="A31" s="58"/>
@@ -1619,7 +1623,7 @@
       </c>
       <c r="E31" s="34"/>
     </row>
-    <row r="32" spans="1:5" ht="36" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="58"/>
       <c r="B32" s="55"/>
       <c r="C32" s="16" t="s">

</xml_diff>

<commit_message>
Add : Notes for node js and code
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E513E3-D17F-4B7C-A395-7B0B3171AF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C7F7DE-1730-45C0-ADD7-162356FCDCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -881,15 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -903,33 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46">
-        <v>1</v>
-      </c>
-      <c r="B5" s="43" t="s">
+      <c r="A5" s="49">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="41" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="47"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="48"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="43">
         <v>2</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="60" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="58" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="55"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="56"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="60">
+      <c r="A20" s="46">
         <v>3</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="49" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="61"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,8 +1505,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="61"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1518,8 +1518,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="47"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1531,8 +1531,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1544,8 +1544,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1557,8 +1557,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1570,8 +1570,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="62"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
@@ -1583,10 +1583,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="57">
+      <c r="A29" s="40">
         <v>4</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1600,8 +1600,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="58"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1613,54 +1613,62 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
       <c r="D31" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="58"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
       <c r="D32" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="E32" s="29"/>
+      <c r="E32" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
       <c r="D33" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E33" s="34"/>
+      <c r="E33" s="34">
+        <v>1</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="59"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
       <c r="D34" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="E34" s="30"/>
+      <c r="E34" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="60">
+      <c r="A35" s="46">
         <v>5</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="49" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1672,8 +1680,8 @@
       <c r="E35" s="26"/>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="61"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1683,8 +1691,8 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="61"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
@@ -1694,8 +1702,8 @@
       <c r="E37" s="32"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="61"/>
-      <c r="B38" s="47"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
@@ -1705,8 +1713,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="61"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
@@ -1716,8 +1724,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="61"/>
-      <c r="B40" s="47"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
@@ -1727,8 +1735,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="61"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1738,8 +1746,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="61"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1749,8 +1757,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="62"/>
-      <c r="B43" s="48"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1760,10 +1768,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="57">
+      <c r="A44" s="40">
         <v>6</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="43" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1775,8 +1783,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="58"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1786,8 +1794,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="55"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="44"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
@@ -1797,8 +1805,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="58"/>
-      <c r="B47" s="55"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1808,8 +1816,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="59"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1819,10 +1827,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="60">
+      <c r="A49" s="46">
         <v>7</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="49" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1834,8 +1842,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="61"/>
-      <c r="B50" s="47"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1845,8 +1853,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="61"/>
-      <c r="B51" s="47"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="50"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1856,8 +1864,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="61"/>
-      <c r="B52" s="47"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1867,8 +1875,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="61"/>
-      <c r="B53" s="47"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1878,8 +1886,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="61"/>
-      <c r="B54" s="47"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1889,8 +1897,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="61"/>
-      <c r="B55" s="47"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1900,8 +1908,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="62"/>
-      <c r="B56" s="48"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1913,6 +1921,13 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1923,13 +1938,6 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes and code for express.js
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C7F7DE-1730-45C0-ADD7-162356FCDCDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB100A0-F9CB-483F-9A90-B5C3558FCECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,15 +923,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,48 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49">
-        <v>1</v>
-      </c>
-      <c r="B5" s="55" t="s">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="51"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="54">
         <v>2</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="51" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="58" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="49" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45"/>
-      <c r="B19" s="62"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
+      <c r="A20" s="60">
         <v>3</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,8 +1505,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1518,8 +1518,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1531,8 +1531,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1544,8 +1544,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1557,8 +1557,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1570,8 +1570,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="48"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
@@ -1583,10 +1583,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40">
+      <c r="A29" s="57">
         <v>4</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="54" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1600,8 +1600,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1613,8 +1613,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
@@ -1626,8 +1626,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
@@ -1639,8 +1639,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1652,8 +1652,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
@@ -1665,10 +1665,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="60">
         <v>5</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="46" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1677,11 +1677,13 @@
       <c r="D35" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E35" s="26"/>
+      <c r="E35" s="26">
+        <v>1</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1691,19 +1693,21 @@
       <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
       <c r="D37" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E37" s="32"/>
+      <c r="E37" s="32">
+        <v>1</v>
+      </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="50"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
@@ -1713,8 +1717,8 @@
       <c r="E38" s="27"/>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
@@ -1724,8 +1728,8 @@
       <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
@@ -1735,8 +1739,8 @@
       <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1746,8 +1750,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1757,8 +1761,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1768,10 +1772,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40">
+      <c r="A44" s="57">
         <v>6</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="54" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1783,8 +1787,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="41"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1794,8 +1798,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="41"/>
-      <c r="B46" s="44"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
@@ -1805,8 +1809,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="41"/>
-      <c r="B47" s="44"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1816,8 +1820,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="42"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="59"/>
+      <c r="B48" s="56"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1827,10 +1831,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="46">
+      <c r="A49" s="60">
         <v>7</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="46" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1842,8 +1846,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="47"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1853,8 +1857,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
-      <c r="B51" s="50"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1864,8 +1868,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="47"/>
-      <c r="B52" s="50"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="47"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1875,8 +1879,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="47"/>
-      <c r="B53" s="50"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1886,8 +1890,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="50"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="47"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1897,8 +1901,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="50"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="47"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1908,8 +1912,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="48"/>
-      <c r="B56" s="51"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1921,13 +1925,6 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1938,6 +1935,13 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Express notes and practiced code
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB100A0-F9CB-483F-9A90-B5C3558FCECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C06A898-2E50-4ADC-9620-3147172C8F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,42 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -881,15 +917,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -903,33 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1215,7 +1215,7 @@
   <dimension ref="A1:E57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="52" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="46">
-        <v>1</v>
-      </c>
-      <c r="B5" s="43" t="s">
+      <c r="A5" s="49">
+        <v>1</v>
+      </c>
+      <c r="B5" s="55" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="47"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="41" t="s">
+      <c r="A6" s="50"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="47"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="42"/>
+      <c r="A7" s="50"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="54"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
-      <c r="B8" s="44"/>
+      <c r="A8" s="50"/>
+      <c r="B8" s="56"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="47"/>
-      <c r="B9" s="44"/>
+      <c r="A9" s="50"/>
+      <c r="B9" s="56"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="47"/>
-      <c r="B10" s="44"/>
+      <c r="A10" s="50"/>
+      <c r="B10" s="56"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="48"/>
-      <c r="B11" s="45"/>
+      <c r="A11" s="51"/>
+      <c r="B11" s="57"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54">
+      <c r="A12" s="43">
         <v>2</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="60" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
-      <c r="B13" s="52"/>
+      <c r="A13" s="44"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="55"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49" t="s">
+      <c r="A14" s="44"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="58" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="55"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="50"/>
+      <c r="A15" s="44"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="59"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="55"/>
-      <c r="B16" s="52"/>
+      <c r="A16" s="44"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="55"/>
-      <c r="B17" s="52"/>
+      <c r="A17" s="44"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="55"/>
-      <c r="B18" s="52"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="56"/>
-      <c r="B19" s="53"/>
+      <c r="A19" s="45"/>
+      <c r="B19" s="62"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="60">
+      <c r="A20" s="46">
         <v>3</v>
       </c>
-      <c r="B20" s="46" t="s">
+      <c r="B20" s="49" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="61"/>
-      <c r="B21" s="47"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="50"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="61"/>
-      <c r="B22" s="47"/>
+      <c r="A22" s="47"/>
+      <c r="B22" s="50"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,8 +1505,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="61"/>
-      <c r="B23" s="47"/>
+      <c r="A23" s="47"/>
+      <c r="B23" s="50"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1518,8 +1518,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="61"/>
-      <c r="B24" s="47"/>
+      <c r="A24" s="47"/>
+      <c r="B24" s="50"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1531,8 +1531,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="61"/>
-      <c r="B25" s="47"/>
+      <c r="A25" s="47"/>
+      <c r="B25" s="50"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1544,8 +1544,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="61"/>
-      <c r="B26" s="47"/>
+      <c r="A26" s="47"/>
+      <c r="B26" s="50"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1557,8 +1557,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="61"/>
-      <c r="B27" s="47"/>
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1570,8 +1570,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="62"/>
-      <c r="B28" s="48"/>
+      <c r="A28" s="48"/>
+      <c r="B28" s="51"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
@@ -1583,10 +1583,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="57">
+      <c r="A29" s="40">
         <v>4</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="43" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1600,8 +1600,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="58"/>
-      <c r="B30" s="55"/>
+      <c r="A30" s="41"/>
+      <c r="B30" s="44"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1613,8 +1613,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="58"/>
-      <c r="B31" s="55"/>
+      <c r="A31" s="41"/>
+      <c r="B31" s="44"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
@@ -1626,8 +1626,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="58"/>
-      <c r="B32" s="55"/>
+      <c r="A32" s="41"/>
+      <c r="B32" s="44"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
@@ -1639,8 +1639,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="55"/>
+      <c r="A33" s="41"/>
+      <c r="B33" s="44"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1652,8 +1652,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="59"/>
-      <c r="B34" s="56"/>
+      <c r="A34" s="42"/>
+      <c r="B34" s="45"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
@@ -1665,10 +1665,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="60">
+      <c r="A35" s="46">
         <v>5</v>
       </c>
-      <c r="B35" s="46" t="s">
+      <c r="B35" s="49" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1682,19 +1682,21 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="61"/>
-      <c r="B36" s="47"/>
+      <c r="A36" s="47"/>
+      <c r="B36" s="50"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="61"/>
-      <c r="B37" s="47"/>
+      <c r="A37" s="47"/>
+      <c r="B37" s="50"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
@@ -1706,41 +1708,47 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="61"/>
-      <c r="B38" s="47"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="50"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
       <c r="D38" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="E38" s="27"/>
+      <c r="E38" s="27">
+        <v>1</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="61"/>
-      <c r="B39" s="47"/>
+      <c r="A39" s="47"/>
+      <c r="B39" s="50"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
       <c r="D39" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="31"/>
+      <c r="E39" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="61"/>
-      <c r="B40" s="47"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="50"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E40" s="31"/>
+      <c r="E40" s="31">
+        <v>1</v>
+      </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="61"/>
-      <c r="B41" s="47"/>
+      <c r="A41" s="47"/>
+      <c r="B41" s="50"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1750,8 +1758,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="61"/>
-      <c r="B42" s="47"/>
+      <c r="A42" s="47"/>
+      <c r="B42" s="50"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1761,8 +1769,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="62"/>
-      <c r="B43" s="48"/>
+      <c r="A43" s="48"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1772,10 +1780,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="57">
+      <c r="A44" s="40">
         <v>6</v>
       </c>
-      <c r="B44" s="54" t="s">
+      <c r="B44" s="43" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1787,8 +1795,8 @@
       <c r="E44" s="33"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="58"/>
-      <c r="B45" s="55"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="44"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1798,8 +1806,8 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="58"/>
-      <c r="B46" s="55"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="44"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
@@ -1809,8 +1817,8 @@
       <c r="E46" s="36"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="58"/>
-      <c r="B47" s="55"/>
+      <c r="A47" s="41"/>
+      <c r="B47" s="44"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1820,8 +1828,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="59"/>
-      <c r="B48" s="56"/>
+      <c r="A48" s="42"/>
+      <c r="B48" s="45"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1831,10 +1839,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="60">
+      <c r="A49" s="46">
         <v>7</v>
       </c>
-      <c r="B49" s="46" t="s">
+      <c r="B49" s="49" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1846,8 +1854,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="61"/>
-      <c r="B50" s="47"/>
+      <c r="A50" s="47"/>
+      <c r="B50" s="50"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1857,8 +1865,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="61"/>
-      <c r="B51" s="47"/>
+      <c r="A51" s="47"/>
+      <c r="B51" s="50"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1868,8 +1876,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="61"/>
-      <c r="B52" s="47"/>
+      <c r="A52" s="47"/>
+      <c r="B52" s="50"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1879,8 +1887,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="61"/>
-      <c r="B53" s="47"/>
+      <c r="A53" s="47"/>
+      <c r="B53" s="50"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1890,8 +1898,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="61"/>
-      <c r="B54" s="47"/>
+      <c r="A54" s="47"/>
+      <c r="B54" s="50"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1901,8 +1909,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="61"/>
-      <c r="B55" s="47"/>
+      <c r="A55" s="47"/>
+      <c r="B55" s="50"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1912,8 +1920,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="62"/>
-      <c r="B56" s="48"/>
+      <c r="A56" s="48"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1925,6 +1933,13 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1935,13 +1950,6 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes for MongoDB
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C06A898-2E50-4ADC-9620-3147172C8F91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC784C8-8219-45FC-B738-AD1C6BA25677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -863,6 +863,57 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -872,15 +923,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -888,48 +930,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1229,13 +1229,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="52" t="s">
+      <c r="A1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
     </row>
     <row r="2" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4"/>
     <row r="3" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
@@ -1263,10 +1263,10 @@
       <c r="E4" s="25"/>
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="49">
-        <v>1</v>
-      </c>
-      <c r="B5" s="55" t="s">
+      <c r="A5" s="46">
+        <v>1</v>
+      </c>
+      <c r="B5" s="43" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1280,9 +1280,9 @@
       </c>
     </row>
     <row r="6" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A6" s="50"/>
-      <c r="B6" s="56"/>
-      <c r="C6" s="53" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="41" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -1293,9 +1293,9 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="50"/>
-      <c r="B7" s="56"/>
-      <c r="C7" s="54"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="42"/>
       <c r="D7" s="7" t="s">
         <v>10</v>
       </c>
@@ -1304,8 +1304,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="50"/>
-      <c r="B8" s="56"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="44"/>
       <c r="C8" s="8" t="s">
         <v>11</v>
       </c>
@@ -1317,8 +1317,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="50"/>
-      <c r="B9" s="56"/>
+      <c r="A9" s="47"/>
+      <c r="B9" s="44"/>
       <c r="C9" s="9" t="s">
         <v>13</v>
       </c>
@@ -1330,8 +1330,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="50"/>
-      <c r="B10" s="56"/>
+      <c r="A10" s="47"/>
+      <c r="B10" s="44"/>
       <c r="C10" s="9" t="s">
         <v>15</v>
       </c>
@@ -1343,8 +1343,8 @@
       </c>
     </row>
     <row r="11" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="51"/>
-      <c r="B11" s="57"/>
+      <c r="A11" s="48"/>
+      <c r="B11" s="45"/>
       <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
@@ -1356,10 +1356,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="43">
+      <c r="A12" s="54">
         <v>2</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="51" t="s">
         <v>20</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -1373,8 +1373,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A13" s="44"/>
-      <c r="B13" s="61"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="52"/>
       <c r="C13" s="16" t="s">
         <v>23</v>
       </c>
@@ -1386,9 +1386,9 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="44"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="58" t="s">
+      <c r="A14" s="55"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="49" t="s">
         <v>25</v>
       </c>
       <c r="D14" s="17" t="s">
@@ -1399,9 +1399,9 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="44"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="59"/>
+      <c r="A15" s="55"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="50"/>
       <c r="D15" s="18" t="s">
         <v>27</v>
       </c>
@@ -1410,8 +1410,8 @@
       </c>
     </row>
     <row r="16" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A16" s="44"/>
-      <c r="B16" s="61"/>
+      <c r="A16" s="55"/>
+      <c r="B16" s="52"/>
       <c r="C16" s="16" t="s">
         <v>28</v>
       </c>
@@ -1423,8 +1423,8 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A17" s="44"/>
-      <c r="B17" s="61"/>
+      <c r="A17" s="55"/>
+      <c r="B17" s="52"/>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
@@ -1436,8 +1436,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A18" s="44"/>
-      <c r="B18" s="61"/>
+      <c r="A18" s="55"/>
+      <c r="B18" s="52"/>
       <c r="C18" s="16" t="s">
         <v>32</v>
       </c>
@@ -1449,8 +1449,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="45"/>
-      <c r="B19" s="62"/>
+      <c r="A19" s="56"/>
+      <c r="B19" s="53"/>
       <c r="C19" s="19" t="s">
         <v>112</v>
       </c>
@@ -1462,10 +1462,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="46">
+      <c r="A20" s="60">
         <v>3</v>
       </c>
-      <c r="B20" s="49" t="s">
+      <c r="B20" s="46" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="7" t="s">
@@ -1479,8 +1479,8 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="47"/>
-      <c r="B21" s="50"/>
+      <c r="A21" s="61"/>
+      <c r="B21" s="47"/>
       <c r="C21" s="10" t="s">
         <v>38</v>
       </c>
@@ -1492,8 +1492,8 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="47"/>
-      <c r="B22" s="50"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="47"/>
       <c r="C22" s="10" t="s">
         <v>40</v>
       </c>
@@ -1505,8 +1505,8 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A23" s="47"/>
-      <c r="B23" s="50"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="47"/>
       <c r="C23" s="10" t="s">
         <v>42</v>
       </c>
@@ -1518,8 +1518,8 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A24" s="47"/>
-      <c r="B24" s="50"/>
+      <c r="A24" s="61"/>
+      <c r="B24" s="47"/>
       <c r="C24" s="10" t="s">
         <v>44</v>
       </c>
@@ -1531,8 +1531,8 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="47"/>
-      <c r="B25" s="50"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="47"/>
       <c r="C25" s="10" t="s">
         <v>45</v>
       </c>
@@ -1544,8 +1544,8 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="47"/>
-      <c r="B26" s="50"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="47"/>
       <c r="C26" s="10" t="s">
         <v>46</v>
       </c>
@@ -1557,8 +1557,8 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="47"/>
-      <c r="B27" s="50"/>
+      <c r="A27" s="61"/>
+      <c r="B27" s="47"/>
       <c r="C27" s="10" t="s">
         <v>48</v>
       </c>
@@ -1570,8 +1570,8 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="48"/>
-      <c r="B28" s="51"/>
+      <c r="A28" s="62"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="12" t="s">
         <v>50</v>
       </c>
@@ -1583,10 +1583,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="40">
+      <c r="A29" s="57">
         <v>4</v>
       </c>
-      <c r="B29" s="43" t="s">
+      <c r="B29" s="54" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="15" t="s">
@@ -1600,8 +1600,8 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A30" s="41"/>
-      <c r="B30" s="44"/>
+      <c r="A30" s="58"/>
+      <c r="B30" s="55"/>
       <c r="C30" s="16" t="s">
         <v>55</v>
       </c>
@@ -1613,8 +1613,8 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
+      <c r="A31" s="58"/>
+      <c r="B31" s="55"/>
       <c r="C31" s="16" t="s">
         <v>58</v>
       </c>
@@ -1626,8 +1626,8 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="41"/>
-      <c r="B32" s="44"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="55"/>
       <c r="C32" s="16" t="s">
         <v>60</v>
       </c>
@@ -1639,8 +1639,8 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="41"/>
-      <c r="B33" s="44"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="55"/>
       <c r="C33" s="16" t="s">
         <v>62</v>
       </c>
@@ -1652,8 +1652,8 @@
       </c>
     </row>
     <row r="34" spans="1:5" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="42"/>
-      <c r="B34" s="45"/>
+      <c r="A34" s="59"/>
+      <c r="B34" s="56"/>
       <c r="C34" s="20" t="s">
         <v>65</v>
       </c>
@@ -1665,10 +1665,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="46">
+      <c r="A35" s="60">
         <v>5</v>
       </c>
-      <c r="B35" s="49" t="s">
+      <c r="B35" s="46" t="s">
         <v>67</v>
       </c>
       <c r="C35" s="5" t="s">
@@ -1682,8 +1682,8 @@
       </c>
     </row>
     <row r="36" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A36" s="47"/>
-      <c r="B36" s="50"/>
+      <c r="A36" s="61"/>
+      <c r="B36" s="47"/>
       <c r="C36" s="10" t="s">
         <v>55</v>
       </c>
@@ -1695,8 +1695,8 @@
       </c>
     </row>
     <row r="37" spans="1:5" ht="54" x14ac:dyDescent="0.35">
-      <c r="A37" s="47"/>
-      <c r="B37" s="50"/>
+      <c r="A37" s="61"/>
+      <c r="B37" s="47"/>
       <c r="C37" s="10" t="s">
         <v>70</v>
       </c>
@@ -1708,8 +1708,8 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="47"/>
-      <c r="B38" s="50"/>
+      <c r="A38" s="61"/>
+      <c r="B38" s="47"/>
       <c r="C38" s="10" t="s">
         <v>72</v>
       </c>
@@ -1721,8 +1721,8 @@
       </c>
     </row>
     <row r="39" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="47"/>
-      <c r="B39" s="50"/>
+      <c r="A39" s="61"/>
+      <c r="B39" s="47"/>
       <c r="C39" s="10" t="s">
         <v>74</v>
       </c>
@@ -1734,8 +1734,8 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="47"/>
-      <c r="B40" s="50"/>
+      <c r="A40" s="61"/>
+      <c r="B40" s="47"/>
       <c r="C40" s="10" t="s">
         <v>76</v>
       </c>
@@ -1747,8 +1747,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="47"/>
-      <c r="B41" s="50"/>
+      <c r="A41" s="61"/>
+      <c r="B41" s="47"/>
       <c r="C41" s="10" t="s">
         <v>78</v>
       </c>
@@ -1758,8 +1758,8 @@
       <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A42" s="47"/>
-      <c r="B42" s="50"/>
+      <c r="A42" s="61"/>
+      <c r="B42" s="47"/>
       <c r="C42" s="10" t="s">
         <v>80</v>
       </c>
@@ -1769,8 +1769,8 @@
       <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="48"/>
-      <c r="B43" s="51"/>
+      <c r="A43" s="62"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="12" t="s">
         <v>82</v>
       </c>
@@ -1780,10 +1780,10 @@
       <c r="E43" s="39"/>
     </row>
     <row r="44" spans="1:5" ht="36.6" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="40">
+      <c r="A44" s="57">
         <v>6</v>
       </c>
-      <c r="B44" s="43" t="s">
+      <c r="B44" s="54" t="s">
         <v>84</v>
       </c>
       <c r="C44" s="15" t="s">
@@ -1792,11 +1792,13 @@
       <c r="D44" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E44" s="33"/>
+      <c r="E44" s="33">
+        <v>1</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="41"/>
-      <c r="B45" s="44"/>
+      <c r="A45" s="58"/>
+      <c r="B45" s="55"/>
       <c r="C45" s="16" t="s">
         <v>87</v>
       </c>
@@ -1806,19 +1808,21 @@
       <c r="E45" s="29"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="41"/>
-      <c r="B46" s="44"/>
+      <c r="A46" s="58"/>
+      <c r="B46" s="55"/>
       <c r="C46" s="16" t="s">
         <v>89</v>
       </c>
       <c r="D46" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="E46" s="36"/>
+      <c r="E46" s="36">
+        <v>1</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="41"/>
-      <c r="B47" s="44"/>
+      <c r="A47" s="58"/>
+      <c r="B47" s="55"/>
       <c r="C47" s="16" t="s">
         <v>91</v>
       </c>
@@ -1828,8 +1832,8 @@
       <c r="E47" s="34"/>
     </row>
     <row r="48" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A48" s="42"/>
-      <c r="B48" s="45"/>
+      <c r="A48" s="59"/>
+      <c r="B48" s="56"/>
       <c r="C48" s="19" t="s">
         <v>93</v>
       </c>
@@ -1839,10 +1843,10 @@
       <c r="E48" s="30"/>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="46">
+      <c r="A49" s="60">
         <v>7</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="46" t="s">
         <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
@@ -1854,8 +1858,8 @@
       <c r="E49" s="26"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="47"/>
-      <c r="B50" s="50"/>
+      <c r="A50" s="61"/>
+      <c r="B50" s="47"/>
       <c r="C50" s="10" t="s">
         <v>98</v>
       </c>
@@ -1865,8 +1869,8 @@
       <c r="E50" s="32"/>
     </row>
     <row r="51" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A51" s="47"/>
-      <c r="B51" s="50"/>
+      <c r="A51" s="61"/>
+      <c r="B51" s="47"/>
       <c r="C51" s="10" t="s">
         <v>100</v>
       </c>
@@ -1876,8 +1880,8 @@
       <c r="E51" s="32"/>
     </row>
     <row r="52" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A52" s="47"/>
-      <c r="B52" s="50"/>
+      <c r="A52" s="61"/>
+      <c r="B52" s="47"/>
       <c r="C52" s="7" t="s">
         <v>102</v>
       </c>
@@ -1887,8 +1891,8 @@
       <c r="E52" s="27"/>
     </row>
     <row r="53" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A53" s="47"/>
-      <c r="B53" s="50"/>
+      <c r="A53" s="61"/>
+      <c r="B53" s="47"/>
       <c r="C53" s="10" t="s">
         <v>104</v>
       </c>
@@ -1898,8 +1902,8 @@
       <c r="E53" s="32"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="47"/>
-      <c r="B54" s="50"/>
+      <c r="A54" s="61"/>
+      <c r="B54" s="47"/>
       <c r="C54" s="10" t="s">
         <v>106</v>
       </c>
@@ -1909,8 +1913,8 @@
       <c r="E54" s="27"/>
     </row>
     <row r="55" spans="1:5" ht="36" x14ac:dyDescent="0.35">
-      <c r="A55" s="47"/>
-      <c r="B55" s="50"/>
+      <c r="A55" s="61"/>
+      <c r="B55" s="47"/>
       <c r="C55" s="10" t="s">
         <v>108</v>
       </c>
@@ -1920,8 +1924,8 @@
       <c r="E55" s="31"/>
     </row>
     <row r="56" spans="1:5" ht="36.6" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A56" s="48"/>
-      <c r="B56" s="51"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="48"/>
       <c r="C56" s="12" t="s">
         <v>110</v>
       </c>
@@ -1933,13 +1937,6 @@
     <row r="57" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="B5:B11"/>
-    <mergeCell ref="A5:A11"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A12:A19"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="B44:B48"/>
     <mergeCell ref="A49:A56"/>
@@ -1950,6 +1947,13 @@
     <mergeCell ref="B29:B34"/>
     <mergeCell ref="A35:A43"/>
     <mergeCell ref="B35:B43"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="B5:B11"/>
+    <mergeCell ref="A5:A11"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="A12:A19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add : Notes for Mongoose and inital setup for React notes
</commit_message>
<xml_diff>
--- a/mern-learning-roadmap.xlsx
+++ b/mern-learning-roadmap.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RishilRamesh\My-Courses\Web-Development-MERN-Stack\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC784C8-8219-45FC-B738-AD1C6BA25677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA788D5-E77B-4C02-A042-983097F9968C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1214,8 +1214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.35"/>
@@ -1805,7 +1805,9 @@
       <c r="D45" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="29">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="58"/>
@@ -1840,7 +1842,9 @@
       <c r="D48" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="30"/>
+      <c r="E48" s="30">
+        <v>1</v>
+      </c>
     </row>
     <row r="49" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A49" s="60">

</xml_diff>